<commit_message>
Removing metadata from .xlsx files
</commit_message>
<xml_diff>
--- a/additional_results_rebuttal/Best_results_comparisons.xlsx
+++ b/additional_results_rebuttal/Best_results_comparisons.xlsx
@@ -2,13 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bodhi91/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631A4CF0-D78B-EA4D-97D3-3768B50C7EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A488B13-6FF2-004A-B5DA-04277180B428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="46">
   <si>
     <t>VTR7 designs</t>
   </si>
@@ -49,9 +44,18 @@
     <t>FPGAPart-VTR</t>
   </si>
   <si>
+    <t>Two dies</t>
+  </si>
+  <si>
+    <t>Geo mean Impr.</t>
+  </si>
+  <si>
     <t>bgm</t>
   </si>
   <si>
+    <t>rWL</t>
+  </si>
+  <si>
     <t>blob_merge</t>
   </si>
   <si>
@@ -61,6 +65,9 @@
     <t>diffeq1</t>
   </si>
   <si>
+    <t>Three dies</t>
+  </si>
+  <si>
     <t>diffeq2</t>
   </si>
   <si>
@@ -71,6 +78,9 @@
   </si>
   <si>
     <t>mcml</t>
+  </si>
+  <si>
+    <t>Four dies</t>
   </si>
   <si>
     <t>mkDelayWorker32B</t>
@@ -339,9 +349,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,6 +365,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -367,11 +383,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -388,6 +416,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -406,17 +435,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,7 +656,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -647,7 +665,7 @@
     <col min="16" max="16" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -665,826 +683,845 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="23" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="23" t="s">
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="25"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="32"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="22"/>
-      <c r="B3" s="26" t="s">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="29"/>
+      <c r="B3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="27" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="26" t="s">
+      <c r="E3" s="35"/>
+      <c r="F3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="27" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="26" t="s">
+      <c r="I3" s="35"/>
+      <c r="J3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="22"/>
-      <c r="L3" s="27" t="s">
+      <c r="K3" s="29"/>
+      <c r="L3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="28"/>
+      <c r="M3" s="35"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N4" s="1"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="30"/>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
+      <c r="O4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7">
+      <c r="P4" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="9">
         <v>591664</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="10">
         <v>585419</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="11">
         <v>44.51</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="12">
         <v>48.89</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="9">
         <v>586332</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="10">
         <v>568438</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="11">
         <v>39.32</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="12">
         <v>39.590000000000003</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="9">
         <v>584236</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="10">
         <v>528162</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="11">
         <v>39.76</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="12">
         <v>39.82</v>
       </c>
       <c r="N5" s="1"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="30"/>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="6" t="s">
+      <c r="O5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="13">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="9">
+        <v>86514</v>
+      </c>
+      <c r="C6" s="10">
+        <v>85914</v>
+      </c>
+      <c r="D6" s="11">
+        <v>105.24</v>
+      </c>
+      <c r="E6" s="12">
+        <v>108.13</v>
+      </c>
+      <c r="F6" s="9">
+        <v>85561</v>
+      </c>
+      <c r="G6" s="10">
+        <v>85272</v>
+      </c>
+      <c r="H6" s="11">
+        <v>99.87</v>
+      </c>
+      <c r="I6" s="12">
+        <v>102.24</v>
+      </c>
+      <c r="J6" s="14">
+        <v>88096</v>
+      </c>
+      <c r="K6" s="11">
+        <v>88914</v>
+      </c>
+      <c r="L6" s="10">
+        <v>102.82</v>
+      </c>
+      <c r="M6" s="15">
+        <v>104.62</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="17">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="9">
+        <v>29501</v>
+      </c>
+      <c r="C7" s="10">
+        <v>28669</v>
+      </c>
+      <c r="D7" s="11">
+        <v>159.46</v>
+      </c>
+      <c r="E7" s="12">
+        <v>162.24</v>
+      </c>
+      <c r="F7" s="9">
+        <v>30490</v>
+      </c>
+      <c r="G7" s="10">
+        <v>28518</v>
+      </c>
+      <c r="H7" s="11">
+        <v>155.15</v>
+      </c>
+      <c r="I7" s="12">
+        <v>157.32900000000001</v>
+      </c>
+      <c r="J7" s="9">
+        <v>30484</v>
+      </c>
+      <c r="K7" s="10">
+        <v>29982</v>
+      </c>
+      <c r="L7" s="11">
+        <v>153.12</v>
+      </c>
+      <c r="M7" s="12">
+        <v>156.24</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="9">
+        <v>9389</v>
+      </c>
+      <c r="C8" s="10">
+        <v>9005</v>
+      </c>
+      <c r="D8" s="11">
+        <v>48.71</v>
+      </c>
+      <c r="E8" s="12">
+        <v>49.12</v>
+      </c>
+      <c r="F8" s="9">
+        <v>9732</v>
+      </c>
+      <c r="G8" s="10">
+        <v>9095</v>
+      </c>
+      <c r="H8" s="11">
+        <v>47.23</v>
+      </c>
+      <c r="I8" s="12">
+        <v>48.16</v>
+      </c>
+      <c r="J8" s="9">
+        <v>9512</v>
+      </c>
+      <c r="K8" s="10">
+        <v>8824</v>
+      </c>
+      <c r="L8" s="10">
+        <v>48.72</v>
+      </c>
+      <c r="M8" s="15">
+        <v>48.68</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="7">
-        <v>86514</v>
-      </c>
-      <c r="C6" s="8">
-        <v>85914</v>
-      </c>
-      <c r="D6" s="9">
-        <v>105.24</v>
-      </c>
-      <c r="E6" s="10">
-        <v>108.13</v>
-      </c>
-      <c r="F6" s="7">
-        <v>85561</v>
-      </c>
-      <c r="G6" s="8">
-        <v>85272</v>
-      </c>
-      <c r="H6" s="9">
-        <v>99.87</v>
-      </c>
-      <c r="I6" s="10">
-        <v>102.24</v>
-      </c>
-      <c r="J6" s="11">
-        <v>88096</v>
-      </c>
-      <c r="K6" s="9">
-        <v>88914</v>
-      </c>
-      <c r="L6" s="8">
-        <v>102.82</v>
-      </c>
-      <c r="M6" s="12">
-        <v>104.62</v>
-      </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="30"/>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="7">
-        <v>29501</v>
-      </c>
-      <c r="C7" s="8">
-        <v>28669</v>
-      </c>
-      <c r="D7" s="9">
-        <v>159.46</v>
-      </c>
-      <c r="E7" s="10">
-        <v>162.24</v>
-      </c>
-      <c r="F7" s="7">
-        <v>30490</v>
-      </c>
-      <c r="G7" s="8">
-        <v>28518</v>
-      </c>
-      <c r="H7" s="9">
-        <v>155.15</v>
-      </c>
-      <c r="I7" s="10">
-        <v>157.32900000000001</v>
-      </c>
-      <c r="J7" s="7">
-        <v>30484</v>
-      </c>
-      <c r="K7" s="8">
-        <v>29982</v>
-      </c>
-      <c r="L7" s="9">
-        <v>153.12</v>
-      </c>
-      <c r="M7" s="10">
-        <v>156.24</v>
-      </c>
-      <c r="N7" s="1"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="30"/>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
+    </row>
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="9">
+        <v>6798</v>
+      </c>
+      <c r="C9" s="10">
+        <v>6721</v>
+      </c>
+      <c r="D9" s="11">
+        <v>60.7</v>
+      </c>
+      <c r="E9" s="12">
+        <v>63.42</v>
+      </c>
+      <c r="F9" s="9">
+        <v>7404</v>
+      </c>
+      <c r="G9" s="10">
+        <v>7172</v>
+      </c>
+      <c r="H9" s="11">
+        <v>64.260000000000005</v>
+      </c>
+      <c r="I9" s="12">
+        <v>66.92</v>
+      </c>
+      <c r="J9" s="9">
+        <v>7424</v>
+      </c>
+      <c r="K9" s="10">
+        <v>7021</v>
+      </c>
+      <c r="L9" s="11">
+        <v>61.72</v>
+      </c>
+      <c r="M9" s="12">
+        <v>62.26</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="7">
-        <v>9389</v>
-      </c>
-      <c r="C8" s="8">
-        <v>9005</v>
-      </c>
-      <c r="D8" s="9">
-        <v>48.71</v>
-      </c>
-      <c r="E8" s="10">
-        <v>49.12</v>
-      </c>
-      <c r="F8" s="7">
-        <v>9732</v>
-      </c>
-      <c r="G8" s="8">
-        <v>9095</v>
-      </c>
-      <c r="H8" s="9">
-        <v>47.23</v>
-      </c>
-      <c r="I8" s="10">
-        <v>48.16</v>
-      </c>
-      <c r="J8" s="7">
-        <v>9512</v>
-      </c>
-      <c r="K8" s="8">
-        <v>8824</v>
-      </c>
-      <c r="L8" s="8">
-        <v>48.72</v>
-      </c>
-      <c r="M8" s="12">
-        <v>48.68</v>
-      </c>
-      <c r="N8" s="1"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="30"/>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="7">
-        <v>6798</v>
-      </c>
-      <c r="C9" s="8">
-        <v>6721</v>
-      </c>
-      <c r="D9" s="9">
-        <v>60.7</v>
-      </c>
-      <c r="E9" s="10">
-        <v>63.42</v>
-      </c>
-      <c r="F9" s="7">
-        <v>7404</v>
-      </c>
-      <c r="G9" s="8">
-        <v>7172</v>
-      </c>
-      <c r="H9" s="9">
-        <v>64.260000000000005</v>
-      </c>
-      <c r="I9" s="10">
-        <v>66.92</v>
-      </c>
-      <c r="J9" s="7">
-        <v>7424</v>
-      </c>
-      <c r="K9" s="8">
-        <v>7021</v>
-      </c>
-      <c r="L9" s="9">
-        <v>61.72</v>
-      </c>
-      <c r="M9" s="10">
-        <v>62.26</v>
-      </c>
-      <c r="N9" s="1"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="30"/>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="7">
+      <c r="P9" s="13">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="9">
         <v>1699741</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="10">
         <v>1671463</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="11">
         <v>9.19</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="12">
         <v>9.6300000000000008</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="9">
         <v>1744322</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="10">
         <v>1723214</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="11">
         <v>9.43</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="12">
         <v>9.9600000000000009</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="9">
         <v>1734159</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="10">
         <v>1732294</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="11">
         <v>9.26</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="12">
         <v>9.33</v>
       </c>
       <c r="N10" s="1"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="30"/>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="7">
+      <c r="O10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" s="17">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="9">
         <v>415688</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="10">
         <v>405419</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="11">
         <v>8.94</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="12">
         <v>9.1199999999999992</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="9">
         <v>412923</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="10">
         <v>412716</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="11">
         <v>9.44</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="12">
         <v>10.19</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="9">
         <v>405426</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="10">
         <v>405331</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="11">
         <v>8.92</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="12">
         <v>9.02</v>
       </c>
       <c r="N11" s="1"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="30"/>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="7">
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="9">
         <v>1124166</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="10">
         <v>1015142</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="11">
         <v>13.71</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="12">
         <v>14.26</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="14">
         <v>1143349</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="11">
         <v>1144356</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="11">
         <v>13.14</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="12">
         <v>14.24</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="9">
         <v>1138352</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="10">
         <v>1134326</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="11">
         <v>13.92</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="12">
         <v>14.62</v>
       </c>
       <c r="N12" s="1"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="30"/>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="7">
+      <c r="O12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="9">
         <v>110496</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="10">
         <v>107548</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="11">
         <v>144.26</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="12">
         <v>146.19999999999999</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="9">
         <v>108944</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="10">
         <v>108542</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="11">
         <v>137.29</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="12">
         <v>139.82</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="9">
         <v>111552</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="10">
         <v>110284</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="11">
         <v>145.24</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="12">
         <v>147.11000000000001</v>
       </c>
       <c r="N13" s="1"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="30"/>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="7">
+      <c r="O13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" s="13">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="9">
         <v>13644</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="10">
         <v>12469</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="11">
         <v>258.24</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="12">
         <v>259.42</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="9">
         <v>13587</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="10">
         <v>12692</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="10">
         <v>245.39</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="15">
         <v>245.23</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="9">
         <v>13462</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="10">
         <v>12821</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="11">
         <v>259.13</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="12">
         <v>260.24</v>
       </c>
       <c r="N14" s="1"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="34"/>
-      <c r="Q14" s="30"/>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="7">
+      <c r="O14" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" s="17">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="9">
         <v>48998</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="10">
         <v>47476</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="11">
         <v>75.19</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="12">
         <v>76.28</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="9">
         <v>50379</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="10">
         <v>46246</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="11">
         <v>71.98</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="12">
         <v>73.260000000000005</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="9">
         <v>50382</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="10">
         <v>50014</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="11">
         <v>74.67</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="12">
         <v>76.92</v>
       </c>
       <c r="N15" s="1"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="30"/>
-    </row>
-    <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="7">
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="9">
         <v>28619</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="10">
         <v>27412</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="11">
         <v>194.69</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="12">
         <v>207.98</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="9">
         <v>27969</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="10">
         <v>25641</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="11">
         <v>212.24</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="12">
         <v>214.31</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="9">
         <v>27826</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16" s="10">
         <v>26143</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="11">
         <v>205.62</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="12">
         <v>206.86</v>
       </c>
       <c r="N16" s="1"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="30"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="11">
+      <c r="A17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="14">
         <v>20984</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="11">
         <v>20994</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="10">
         <v>79.62</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="15">
         <v>78.239999999999995</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="14">
         <v>22034</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="11">
         <v>22647</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="10">
         <v>79.290000000000006</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="15">
         <v>76.239999999999995</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="9">
         <v>22172</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17" s="10">
         <v>20478</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="11">
         <v>73.62</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="12">
         <v>74.239999999999995</v>
       </c>
       <c r="N17" s="1"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="30"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="7">
+      <c r="A18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="9">
         <v>90426</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="10">
         <v>90014</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="11">
         <v>244.15</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="12">
         <v>262.10000000000002</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="9">
         <v>93553</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="10">
         <v>92393</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="11">
         <v>245.19</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="12">
         <v>246.42</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="9">
         <v>97298</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K18" s="10">
         <v>90684</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="11">
         <v>246.38</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="12">
         <v>247.78</v>
       </c>
       <c r="N18" s="1"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="30"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="7">
+      <c r="A19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="9">
         <v>160512</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="10">
         <v>154126</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="11">
         <v>177.51</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="12">
         <v>186.79</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="9">
         <v>161302</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="10">
         <v>160671</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="11">
         <v>179.28</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="12">
         <v>179.98</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="9">
         <v>167649</v>
       </c>
-      <c r="K19" s="8">
+      <c r="K19" s="10">
         <v>153552</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="11">
         <v>175.24</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="12">
         <v>179.92</v>
       </c>
       <c r="N19" s="1"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="30"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
     </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="14">
+      <c r="A20" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="20">
         <v>843896</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="21">
         <v>807082</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="22">
         <v>62.19</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="23">
         <v>67.42</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="20">
         <v>798888</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="21">
         <v>734728</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="22">
         <v>57.82</v>
       </c>
-      <c r="I20" s="17">
+      <c r="I20" s="23">
         <v>62.24</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="20">
         <v>823214</v>
       </c>
-      <c r="K20" s="15">
+      <c r="K20" s="21">
         <v>720019</v>
       </c>
-      <c r="L20" s="16">
+      <c r="L20" s="22">
         <v>62.19</v>
       </c>
-      <c r="M20" s="17">
+      <c r="M20" s="23">
         <v>63.39</v>
       </c>
       <c r="N20" s="1"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="30"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
@@ -1501,691 +1538,724 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="30"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="23" t="s">
+      <c r="A22" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="23" t="s">
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="23" t="s">
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="25"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="32"/>
       <c r="N22" s="1"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
-      <c r="Q22" s="30"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="22"/>
-      <c r="B23" s="26" t="s">
+      <c r="A23" s="29"/>
+      <c r="B23" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="27" t="s">
+      <c r="C23" s="29"/>
+      <c r="D23" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="26" t="s">
+      <c r="E23" s="35"/>
+      <c r="F23" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="22"/>
-      <c r="H23" s="27" t="s">
+      <c r="G23" s="29"/>
+      <c r="H23" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I23" s="28"/>
-      <c r="J23" s="26" t="s">
+      <c r="I23" s="35"/>
+      <c r="J23" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="K23" s="22"/>
-      <c r="L23" s="27" t="s">
+      <c r="K23" s="29"/>
+      <c r="L23" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="M23" s="28"/>
+      <c r="M23" s="35"/>
       <c r="N23" s="1"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="32"/>
-      <c r="Q23" s="30"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="L24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M24" s="5" t="s">
+      <c r="M24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N24" s="19"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="33"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="26"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="7">
+      <c r="A25" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="9">
         <v>2296992</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="10">
         <v>2222412</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="11">
         <v>85.12</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="12">
         <v>86.24</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="9">
         <v>2366846</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="10">
         <v>2223648</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="11">
         <v>85.21</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="12">
         <v>87.33</v>
       </c>
-      <c r="J25" s="7">
+      <c r="J25" s="9">
         <v>2264318</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K25" s="10">
         <v>1974646</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25" s="11">
         <v>87.21</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M25" s="12">
         <v>89.95</v>
       </c>
-      <c r="N25" s="19"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="33"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="26"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="7">
+      <c r="A26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="9">
         <v>489862</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="10">
         <v>467824</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="11">
         <v>90.69</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="12">
         <v>95.12</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="14">
         <v>553687</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="11">
         <v>586214</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="11">
         <v>79.19</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="12">
         <v>88.24</v>
       </c>
-      <c r="J26" s="11">
+      <c r="J26" s="14">
         <v>456844</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="11">
         <v>461474</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L26" s="11">
         <v>79.680000000000007</v>
       </c>
-      <c r="M26" s="10">
+      <c r="M26" s="12">
         <v>85.92</v>
       </c>
-      <c r="N26" s="19"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
-      <c r="Q26" s="33"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q26" s="26"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="7">
+      <c r="A27" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="9">
         <v>4016482</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="10">
         <v>4012624</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="11">
         <v>69.319999999999993</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="12">
         <v>81.88</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="9">
         <v>4198486</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="10">
         <v>4169832</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="11">
         <v>83.96</v>
       </c>
-      <c r="I27" s="10">
+      <c r="I27" s="12">
         <v>86.19</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J27" s="9">
         <v>4364426</v>
       </c>
-      <c r="K27" s="8">
+      <c r="K27" s="10">
         <v>4048462</v>
       </c>
-      <c r="L27" s="9">
+      <c r="L27" s="11">
         <v>82.71</v>
       </c>
-      <c r="M27" s="10">
+      <c r="M27" s="12">
         <v>85.32</v>
       </c>
-      <c r="N27" s="19"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="34"/>
-      <c r="Q27" s="33"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P27" s="13">
+        <v>0.04</v>
+      </c>
+      <c r="Q27" s="26"/>
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="11">
+      <c r="A28" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="14">
         <v>1634662</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="11">
         <v>1656796</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="11">
         <v>108.14</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="12">
         <v>109.19</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="9">
         <v>1662143</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="10">
         <v>1636431</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="11">
         <v>111.2</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="12">
         <v>114.62</v>
       </c>
-      <c r="J28" s="7">
+      <c r="J28" s="9">
         <v>1652674</v>
       </c>
-      <c r="K28" s="8">
+      <c r="K28" s="10">
         <v>1510798</v>
       </c>
-      <c r="L28" s="9">
+      <c r="L28" s="11">
         <v>106.51</v>
       </c>
-      <c r="M28" s="10">
+      <c r="M28" s="12">
         <v>109.92</v>
       </c>
-      <c r="N28" s="19"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="33"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="P28" s="17">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="Q28" s="26"/>
     </row>
     <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="7">
+      <c r="A29" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="9">
         <v>102242</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="10">
         <v>94546</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="11">
         <v>108.21</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="12">
         <v>112.26</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="9">
         <v>101428</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="10">
         <v>87246</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="11">
         <v>110.16</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29" s="12">
         <v>128.41999999999999</v>
       </c>
-      <c r="J29" s="7">
+      <c r="J29" s="9">
         <v>108162</v>
       </c>
-      <c r="K29" s="8">
+      <c r="K29" s="10">
         <v>80247</v>
       </c>
-      <c r="L29" s="9">
+      <c r="L29" s="11">
         <v>113.25</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M29" s="12">
         <v>121.26</v>
       </c>
-      <c r="N29" s="19"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="33"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="26"/>
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="11">
+      <c r="A30" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="14">
         <v>1286428</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="11">
         <v>1342682</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="11">
         <v>91.12</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="12">
         <v>94.84</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="9">
         <v>1384321</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="10">
         <v>1333624</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="11">
         <v>96.39</v>
       </c>
-      <c r="I30" s="10">
+      <c r="I30" s="12">
         <v>101.26</v>
       </c>
-      <c r="J30" s="7">
+      <c r="J30" s="9">
         <v>1321077</v>
       </c>
-      <c r="K30" s="8">
+      <c r="K30" s="10">
         <v>1244639</v>
       </c>
-      <c r="L30" s="9">
+      <c r="L30" s="11">
         <v>94.12</v>
       </c>
-      <c r="M30" s="10">
+      <c r="M30" s="12">
         <v>96.37</v>
       </c>
-      <c r="N30" s="19"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
-      <c r="Q30" s="33"/>
+      <c r="N30" s="25"/>
+      <c r="O30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P30" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q30" s="26"/>
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="7">
+      <c r="A31" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="9">
         <v>184864</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="10">
         <v>174485</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="11">
         <v>212.56</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="12">
         <v>216.72</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="9">
         <v>184352</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="10">
         <v>171095</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="11">
         <v>209.42</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I31" s="12">
         <v>216.39</v>
       </c>
-      <c r="J31" s="7">
+      <c r="J31" s="9">
         <v>193694</v>
       </c>
-      <c r="K31" s="8">
+      <c r="K31" s="10">
         <v>179528</v>
       </c>
-      <c r="L31" s="9">
+      <c r="L31" s="11">
         <v>195.28</v>
       </c>
-      <c r="M31" s="10">
+      <c r="M31" s="12">
         <v>214.19</v>
       </c>
-      <c r="N31" s="19"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="34"/>
-      <c r="Q31" s="33"/>
+      <c r="N31" s="25"/>
+      <c r="O31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P31" s="13">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="Q31" s="26"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="11">
+      <c r="A32" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="14">
         <v>215544</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="11">
         <v>216442</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="10">
         <v>110.13</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="15">
         <v>109.23</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="9">
         <v>214624</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="10">
         <v>214036</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="11">
         <v>111.24</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="12">
         <v>111.96</v>
       </c>
-      <c r="J32" s="11">
+      <c r="J32" s="14">
         <v>232264</v>
       </c>
-      <c r="K32" s="9">
+      <c r="K32" s="11">
         <v>232514</v>
       </c>
-      <c r="L32" s="9">
+      <c r="L32" s="11">
         <v>97.47</v>
       </c>
-      <c r="M32" s="10">
+      <c r="M32" s="12">
         <v>111.42</v>
       </c>
-      <c r="N32" s="19"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="34"/>
-      <c r="Q32" s="33"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="P32" s="17">
+        <v>3.1E-2</v>
+      </c>
+      <c r="Q32" s="26"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="7">
+      <c r="A33" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="9">
         <v>2104664</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="10">
         <v>1814268</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="11">
         <v>96.88</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="12">
         <v>105.22</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="9">
         <v>2042162</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="10">
         <v>2033215</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="11">
         <v>88.39</v>
       </c>
-      <c r="I33" s="10">
+      <c r="I33" s="12">
         <v>94.17</v>
       </c>
-      <c r="J33" s="7">
+      <c r="J33" s="9">
         <v>2103329</v>
       </c>
-      <c r="K33" s="8">
+      <c r="K33" s="10">
         <v>1865124</v>
       </c>
-      <c r="L33" s="9">
+      <c r="L33" s="11">
         <v>83.56</v>
       </c>
-      <c r="M33" s="10">
+      <c r="M33" s="12">
         <v>99.13</v>
       </c>
-      <c r="N33" s="19"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="31"/>
-      <c r="Q33" s="33"/>
+      <c r="N33" s="25"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="26"/>
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="7">
+      <c r="A34" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="9">
         <v>167462</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="10">
         <v>153486</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="11">
         <v>135.79</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="12">
         <v>138.63</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="9">
         <v>159521</v>
       </c>
-      <c r="G34" s="8">
+      <c r="G34" s="10">
         <v>159014</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H34" s="11">
         <v>135.47999999999999</v>
       </c>
-      <c r="I34" s="10">
+      <c r="I34" s="12">
         <v>139.1</v>
       </c>
-      <c r="J34" s="7">
+      <c r="J34" s="9">
         <v>162525</v>
       </c>
-      <c r="K34" s="8">
+      <c r="K34" s="10">
         <v>143653</v>
       </c>
-      <c r="L34" s="9">
+      <c r="L34" s="11">
         <v>144.43</v>
       </c>
-      <c r="M34" s="10">
+      <c r="M34" s="12">
         <v>147.93</v>
       </c>
-      <c r="N34" s="19"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="31"/>
-      <c r="Q34" s="33"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P34" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q34" s="26"/>
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="7">
+      <c r="A35" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="9">
         <v>210556</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="10">
         <v>203058</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="11">
         <v>99.21</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="12">
         <v>100.1</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="9">
         <v>216435</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="10">
         <v>205436</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H35" s="11">
         <v>99.19</v>
       </c>
-      <c r="I35" s="10">
+      <c r="I35" s="12">
         <v>99.24</v>
       </c>
-      <c r="J35" s="7">
+      <c r="J35" s="9">
         <v>227246</v>
       </c>
-      <c r="K35" s="8">
+      <c r="K35" s="10">
         <v>200562</v>
       </c>
-      <c r="L35" s="9">
+      <c r="L35" s="11">
         <v>95.61</v>
       </c>
-      <c r="M35" s="10">
+      <c r="M35" s="12">
         <v>99.26</v>
       </c>
-      <c r="N35" s="19"/>
-      <c r="O35" s="31"/>
-      <c r="P35" s="34"/>
-      <c r="Q35" s="33"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P35" s="13">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="Q35" s="26"/>
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="11">
+      <c r="A36" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="14">
         <v>170342</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="11">
         <v>170366</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="11">
         <v>152.41999999999999</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="12">
         <v>155.36000000000001</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="9">
         <v>174246</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="10">
         <v>167532</v>
       </c>
-      <c r="H36" s="9">
+      <c r="H36" s="11">
         <v>157.62</v>
       </c>
-      <c r="I36" s="10">
+      <c r="I36" s="12">
         <v>159.24</v>
       </c>
-      <c r="J36" s="7">
+      <c r="J36" s="9">
         <v>175347</v>
       </c>
-      <c r="K36" s="8">
+      <c r="K36" s="10">
         <v>153465</v>
       </c>
-      <c r="L36" s="9">
+      <c r="L36" s="11">
         <v>151.78</v>
       </c>
-      <c r="M36" s="10">
+      <c r="M36" s="12">
         <v>155.26</v>
       </c>
-      <c r="N36" s="19"/>
-      <c r="O36" s="31"/>
-      <c r="P36" s="34"/>
-      <c r="Q36" s="33"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="P36" s="17">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="Q36" s="26"/>
     </row>
     <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="7">
+      <c r="A37" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="9">
         <v>222481</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="10">
         <v>212864</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="11">
         <v>154.31</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="12">
         <v>156.72</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="9">
         <v>233058</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G37" s="10">
         <v>224616</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H37" s="10">
         <v>141.41999999999999</v>
       </c>
-      <c r="I37" s="12">
+      <c r="I37" s="15">
         <v>139.38999999999999</v>
       </c>
-      <c r="J37" s="7">
+      <c r="J37" s="9">
         <v>275619</v>
       </c>
-      <c r="K37" s="8">
+      <c r="K37" s="10">
         <v>226414</v>
       </c>
-      <c r="L37" s="9">
+      <c r="L37" s="11">
         <v>143.29</v>
       </c>
-      <c r="M37" s="10">
+      <c r="M37" s="12">
         <v>146.93</v>
       </c>
       <c r="N37" s="1"/>
@@ -2193,43 +2263,43 @@
       <c r="P37" s="1"/>
     </row>
     <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="7">
+      <c r="A38" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="9">
         <v>464263</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="10">
         <v>445674</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="11">
         <v>138.91999999999999</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38" s="12">
         <v>138.97999999999999</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="9">
         <v>442062</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="10">
         <v>337602</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H38" s="11">
         <v>142.36000000000001</v>
       </c>
-      <c r="I38" s="10">
+      <c r="I38" s="12">
         <v>148.55000000000001</v>
       </c>
-      <c r="J38" s="7">
+      <c r="J38" s="9">
         <v>451263</v>
       </c>
-      <c r="K38" s="8">
+      <c r="K38" s="10">
         <v>393298</v>
       </c>
-      <c r="L38" s="9">
+      <c r="L38" s="11">
         <v>139.1</v>
       </c>
-      <c r="M38" s="10">
+      <c r="M38" s="12">
         <v>147.25</v>
       </c>
       <c r="N38" s="1"/>
@@ -2237,43 +2307,43 @@
       <c r="P38" s="1"/>
     </row>
     <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="14">
+      <c r="A39" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="20">
         <v>448432</v>
       </c>
-      <c r="C39" s="15">
+      <c r="C39" s="21">
         <v>431542</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="22">
         <v>104.95</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="23">
         <v>105.26</v>
       </c>
-      <c r="F39" s="14">
+      <c r="F39" s="20">
         <v>440418</v>
       </c>
-      <c r="G39" s="15">
+      <c r="G39" s="21">
         <v>406520</v>
       </c>
-      <c r="H39" s="16">
+      <c r="H39" s="22">
         <v>101.19</v>
       </c>
-      <c r="I39" s="17">
+      <c r="I39" s="23">
         <v>108.19</v>
       </c>
-      <c r="J39" s="14">
+      <c r="J39" s="20">
         <v>453284</v>
       </c>
-      <c r="K39" s="15">
+      <c r="K39" s="21">
         <v>422546</v>
       </c>
-      <c r="L39" s="16">
+      <c r="L39" s="22">
         <v>87.92</v>
       </c>
-      <c r="M39" s="17">
+      <c r="M39" s="23">
         <v>101.23</v>
       </c>
       <c r="N39" s="1"/>

</xml_diff>